<commit_message>
modified:   iAdams.m 	modified:   p1_1.eps 	modified:   p1_1.m 	modified:   p1_1.xlsx 	modified:   p1_2.eps 	modified:   p1_2.m 	modified:   p1_2.xlsx 	new file:   p2_1.m 	new file:   p2_1solve.m 	modified:   result1-1.xlsx 	modified:   result1-2.xlsx
</commit_message>
<xml_diff>
--- a/p1_1.xlsx
+++ b/p1_1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,17 +10,17 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398D8FFB-FE02-4E1A-BB34-7A428F9518BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26730" yWindow="20070" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26730" yWindow="20070" windowWidth="19200" windowHeight="11170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -41,7 +41,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -49,12 +49,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -73,7 +75,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -224,7 +226,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -248,9 +250,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -274,7 +276,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -309,7 +311,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -327,7 +329,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -352,7 +354,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -368,104 +370,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="2" width="13.08984375" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" customWidth="true"/>
+    <col min="3" max="3" width="12.453125" customWidth="true"/>
+    <col min="4" max="4" width="13.08984375" customWidth="true"/>
+    <col min="5" max="5" width="14.08984375" customWidth="true"/>
+    <col min="2" max="2" width="13.08984375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1">
+    <row r="1">
+      <c r="A1" s="0">
         <v>10</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="0">
         <v>20</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="0">
         <v>40</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="0">
         <v>60</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="0">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>-0.18774054312323901</v>
-      </c>
-      <c r="B2">
-        <v>-0.58895837354868874</v>
-      </c>
-      <c r="C2">
-        <v>0.30375195751786227</v>
-      </c>
-      <c r="D2">
-        <v>-0.30549599943113331</v>
-      </c>
-      <c r="E2">
-        <v>-7.8492526880066901E-2</v>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>-0.18831388744517291</v>
+      </c>
+      <c r="B2" s="0">
+        <v>-0.58941692700257031</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0.30365503262274862</v>
+      </c>
+      <c r="D2" s="0">
+        <v>-0.30584205623914329</v>
+      </c>
+      <c r="E2" s="0">
+        <v>-0.078780860491483265</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>-0.20747092935685243</v>
-      </c>
-      <c r="B3">
-        <v>-0.63127747500175946</v>
-      </c>
-      <c r="C3">
-        <v>0.3176709780219466</v>
-      </c>
-      <c r="D3">
-        <v>-0.32085651931705622</v>
-      </c>
-      <c r="E3">
-        <v>-7.8156416177965676E-2</v>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>-0.20810107090629623</v>
+      </c>
+      <c r="B3" s="0">
+        <v>-0.63178884480325992</v>
+      </c>
+      <c r="C3" s="0">
+        <v>0.31756122672862419</v>
+      </c>
+      <c r="D3" s="0">
+        <v>-0.3212316741614169</v>
+      </c>
+      <c r="E3" s="0">
+        <v>-0.078464282939658375</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>-0.71400951818017977</v>
-      </c>
-      <c r="B4">
-        <v>-0.32316388775135729</v>
-      </c>
-      <c r="C4">
-        <v>0.26117509878109441</v>
-      </c>
-      <c r="D4">
-        <v>-0.5238366475593661</v>
-      </c>
-      <c r="E4">
-        <v>-0.62341717666721352</v>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>-0.71373338202181469</v>
+      </c>
+      <c r="B4" s="0">
+        <v>-0.32267450327747688</v>
+      </c>
+      <c r="C4" s="0">
+        <v>0.26062939509323396</v>
+      </c>
+      <c r="D4" s="0">
+        <v>-0.52379545683380802</v>
+      </c>
+      <c r="E4" s="0">
+        <v>-0.62344581981811453</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>-0.77508088798362063</v>
-      </c>
-      <c r="B5">
-        <v>-0.36425847237142295</v>
-      </c>
-      <c r="C5">
-        <v>0.2757950924189464</v>
-      </c>
-      <c r="D5">
-        <v>-0.56462253138396135</v>
-      </c>
-      <c r="E5">
-        <v>-0.66398954847300928</v>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>-0.77478761137803376</v>
+      </c>
+      <c r="B5" s="0">
+        <v>-0.36374971582050242</v>
+      </c>
+      <c r="C5" s="0">
+        <v>0.27519400160685986</v>
+      </c>
+      <c r="D5" s="0">
+        <v>-0.56459947019063006</v>
+      </c>
+      <c r="E5" s="0">
+        <v>-0.66403069789680547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   iAdams.m 	modified:   p1_1.eps 	modified:   p1_1.xlsx 	modified:   p1_2.eps 	modified:   p1_2.xlsx 	modified:   p3.eps 	modified:   p3.m 	modified:   p3.xlsx 	new file:   p4.m 	new file:   p4bx.m 	new file:   p4solve.m 	modified:   result1-1.xlsx 	modified:   result1-2.xlsx 	modified:   result3.xlsx
</commit_message>
<xml_diff>
--- a/p1_1.xlsx
+++ b/p1_1.xlsx
@@ -405,70 +405,70 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>-0.18831388744517291</v>
+        <v>-0.1883138874451831</v>
       </c>
       <c r="B2" s="0">
-        <v>-0.58941692700257031</v>
+        <v>-0.5894169270025974</v>
       </c>
       <c r="C2" s="0">
-        <v>0.30365503262274862</v>
+        <v>0.30365503262272042</v>
       </c>
       <c r="D2" s="0">
-        <v>-0.30584205623914329</v>
+        <v>-0.30584205623916055</v>
       </c>
       <c r="E2" s="0">
-        <v>-0.078780860491483265</v>
+        <v>-0.078780860491486637</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>-0.20810107090629623</v>
+        <v>-0.20810107090631194</v>
       </c>
       <c r="B3" s="0">
-        <v>-0.63178884480325992</v>
+        <v>-0.631788844803293</v>
       </c>
       <c r="C3" s="0">
-        <v>0.31756122672862419</v>
+        <v>0.31756122672858977</v>
       </c>
       <c r="D3" s="0">
-        <v>-0.3212316741614169</v>
+        <v>-0.32123167416143589</v>
       </c>
       <c r="E3" s="0">
-        <v>-0.078464282939658375</v>
+        <v>-0.078464282939662136</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>-0.71373338202181469</v>
+        <v>-0.71373338202149772</v>
       </c>
       <c r="B4" s="0">
-        <v>-0.32267450327747688</v>
+        <v>-0.3226745032772726</v>
       </c>
       <c r="C4" s="0">
-        <v>0.26062939509323396</v>
+        <v>0.26062939509331251</v>
       </c>
       <c r="D4" s="0">
-        <v>-0.52379545683380802</v>
+        <v>-0.52379545683377948</v>
       </c>
       <c r="E4" s="0">
-        <v>-0.62344581981811453</v>
+        <v>-0.62344581981811387</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>-0.77478761137803376</v>
+        <v>-0.77478761137767871</v>
       </c>
       <c r="B5" s="0">
-        <v>-0.36374971582050242</v>
+        <v>-0.36374971582027726</v>
       </c>
       <c r="C5" s="0">
-        <v>0.27519400160685986</v>
+        <v>0.27519400160695306</v>
       </c>
       <c r="D5" s="0">
-        <v>-0.56459947019063006</v>
+        <v>-0.5645994701906033</v>
       </c>
       <c r="E5" s="0">
-        <v>-0.66403069789680547</v>
+        <v>-0.66403069789680502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>